<commit_message>
fix: layouts and role management try #1
</commit_message>
<xml_diff>
--- a/public/academicos.xlsx
+++ b/public/academicos.xlsx
@@ -22,19 +22,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
-    <t xml:space="preserve">Jerimundo silva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teste2@gmail.com</t>
+    <t xml:space="preserve">Jeremiahs silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teste3@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">admin123</t>
   </si>
   <si>
-    <t xml:space="preserve">Amarildo bastos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teste@gmail.com</t>
+    <t xml:space="preserve">Vilinda bastos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teste4@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -255,7 +255,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -275,7 +275,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>100032659</v>
+        <v>100033659</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -289,13 +289,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>100023987</v>
+        <v>100023887</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="teste2@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="teste@gmail.com"/>
+    <hyperlink ref="B1" r:id="rId1" display="teste3@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="teste4@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>